<commit_message>
Add BDD history for SpreadsheetFetcher
</commit_message>
<xml_diff>
--- a/src/test/resources/files/rawdata.xlsx
+++ b/src/test/resources/files/rawdata.xlsx
@@ -13,8 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
-    <sheet name="ITUA" sheetId="2" r:id="rId2"/>
-    <sheet name="ITUE" sheetId="4" r:id="rId3"/>
+    <sheet name="ITUA-Raw" sheetId="2" r:id="rId2"/>
+    <sheet name="ITUA-IMPUTED" sheetId="4" r:id="rId3"/>
     <sheet name="Indicator-NORMALISED" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>

</xml_diff>